<commit_message>
two mails columns added, now should easily work, tests more precised
</commit_message>
<xml_diff>
--- a/tests/test_parsing.xlsx
+++ b/tests/test_parsing.xlsx
@@ -61,7 +61,23 @@
     <t>Evie Delarosa</t>
   </si>
   <si>
-    <t>dan.taylor@rediffmail.com</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>dan.taylor@rediffmail.com;;cos@</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>rediffmail.com</t>
+    </r>
   </si>
   <si>
     <t>Osiris Webster</t>
@@ -169,7 +185,7 @@
     <t>Kobe Peck</t>
   </si>
   <si>
-    <t>uc5semub3428tym98a@ymail.com</t>
+    <t>uc5semub3428tym98a@ymail.com;zas@nromalna</t>
   </si>
   <si>
     <t>Crystal Rosario</t>
@@ -214,7 +230,7 @@
     <t>Miguel Lowery</t>
   </si>
   <si>
-    <t>yxu5zetwias4@rediffmail.com</t>
+    <t>yxu5zetwias4@rediffmail.com;normalnie@cos</t>
   </si>
   <si>
     <t>Estelle Cisneros</t>
@@ -1070,7 +1086,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1095,6 +1111,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1254,7 +1276,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1331,6 +1353,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -10775,6 +10798,16 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G5" r:id="rId2" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G6" r:id="rId3" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G7" r:id="rId4" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G8" r:id="rId5" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G9" r:id="rId6" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G10" r:id="rId7" location="" tooltip="" display="rediffmail.com"/>
+    <hyperlink ref="G11" r:id="rId8" location="" tooltip="" display="rediffmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>